<commit_message>
Fixed Invoke workflow errors
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\harih\OneDrive\Documents\UiPath\PayablesManager\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\testb\Documents\UiPath\FederalBotFactory\PayablesManager\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0082ADC0-9A80-4ACD-ABD8-D13B6546E77E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B56025C-8B06-41B0-9D6A-CBF40C02E768}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="468" uniqueCount="349">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="470" uniqueCount="350">
   <si>
     <t>Name</t>
   </si>
@@ -949,9 +949,6 @@
     <t>Failed - System Exception</t>
   </si>
   <si>
-    <t>Output</t>
-  </si>
-  <si>
     <t>TimeOut_HandleSecurityWarnings_Continue</t>
   </si>
   <si>
@@ -1074,6 +1071,12 @@
   </si>
   <si>
     <t>Refer logs for additional info</t>
+  </si>
+  <si>
+    <t>PayablesManager_</t>
+  </si>
+  <si>
+    <t>TimeOut_IEModeEdgeBrowser</t>
   </si>
 </sst>
 </file>
@@ -1139,36 +1142,32 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+  <cellXfs count="13">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1483,10 +1482,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Z1044"/>
+  <dimension ref="A1:Z1046"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A134" workbookViewId="0">
-      <selection activeCell="A149" sqref="A149"/>
+    <sheetView tabSelected="1" topLeftCell="A72" workbookViewId="0">
+      <selection activeCell="G89" sqref="G89"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1"/>
@@ -1578,10 +1577,10 @@
       </c>
     </row>
     <row r="8" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A8" s="10" t="s">
+      <c r="A8" t="s">
         <v>159</v>
       </c>
-      <c r="B8" s="10">
+      <c r="B8">
         <v>0</v>
       </c>
       <c r="C8" t="s">
@@ -1589,11 +1588,11 @@
       </c>
     </row>
     <row r="9" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="10" spans="1:26" s="10" customFormat="1" ht="14.25" customHeight="1">
-      <c r="A10" s="14" t="s">
+    <row r="10" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A10" s="2" t="s">
         <v>162</v>
       </c>
-      <c r="B10" s="15" t="s">
+      <c r="B10" s="11" t="s">
         <v>163</v>
       </c>
     </row>
@@ -1607,82 +1606,82 @@
     </row>
     <row r="12" spans="1:26" ht="14.5">
       <c r="A12" t="s">
+        <v>323</v>
+      </c>
+      <c r="B12" t="s">
         <v>324</v>
-      </c>
-      <c r="B12" t="s">
-        <v>325</v>
       </c>
     </row>
     <row r="13" spans="1:26" ht="14.5">
       <c r="A13" t="s">
+        <v>325</v>
+      </c>
+      <c r="B13" t="s">
         <v>326</v>
-      </c>
-      <c r="B13" t="s">
-        <v>327</v>
       </c>
     </row>
     <row r="14" spans="1:26" ht="14.5">
       <c r="A14" t="s">
+        <v>327</v>
+      </c>
+      <c r="B14" t="s">
         <v>328</v>
-      </c>
-      <c r="B14" t="s">
-        <v>329</v>
       </c>
     </row>
     <row r="15" spans="1:26" ht="14.5">
       <c r="A15" t="s">
+        <v>329</v>
+      </c>
+      <c r="B15" t="s">
         <v>330</v>
-      </c>
-      <c r="B15" t="s">
-        <v>331</v>
       </c>
     </row>
     <row r="16" spans="1:26" ht="14.5">
       <c r="A16" t="s">
+        <v>341</v>
+      </c>
+      <c r="B16" t="s">
         <v>342</v>
-      </c>
-      <c r="B16" t="s">
-        <v>343</v>
       </c>
     </row>
     <row r="17" spans="1:3" ht="14.5">
       <c r="A17" t="s">
+        <v>331</v>
+      </c>
+      <c r="B17" t="s">
         <v>332</v>
-      </c>
-      <c r="B17" t="s">
-        <v>333</v>
       </c>
     </row>
     <row r="18" spans="1:3" ht="14.5">
       <c r="A18" t="s">
+        <v>333</v>
+      </c>
+      <c r="B18" t="s">
         <v>334</v>
-      </c>
-      <c r="B18" t="s">
-        <v>335</v>
       </c>
     </row>
     <row r="19" spans="1:3" ht="14.5">
       <c r="A19" t="s">
+        <v>335</v>
+      </c>
+      <c r="B19" t="s">
         <v>336</v>
-      </c>
-      <c r="B19" t="s">
-        <v>337</v>
       </c>
     </row>
     <row r="20" spans="1:3" ht="14.5">
       <c r="A20" t="s">
+        <v>337</v>
+      </c>
+      <c r="B20" t="s">
         <v>338</v>
-      </c>
-      <c r="B20" t="s">
-        <v>339</v>
       </c>
     </row>
     <row r="21" spans="1:3" ht="14.5">
       <c r="A21" t="s">
+        <v>339</v>
+      </c>
+      <c r="B21" t="s">
         <v>340</v>
-      </c>
-      <c r="B21" t="s">
-        <v>341</v>
       </c>
     </row>
     <row r="22" spans="1:3" ht="14.25" customHeight="1">
@@ -1703,10 +1702,10 @@
     </row>
     <row r="24" spans="1:3" ht="14.5">
       <c r="A24" t="s">
+        <v>344</v>
+      </c>
+      <c r="B24" t="s">
         <v>345</v>
-      </c>
-      <c r="B24" t="s">
-        <v>346</v>
       </c>
     </row>
     <row r="25" spans="1:3" ht="14.5"/>
@@ -1965,7 +1964,7 @@
       <c r="A62" t="s">
         <v>170</v>
       </c>
-      <c r="B62" s="5" t="s">
+      <c r="B62" t="s">
         <v>60</v>
       </c>
     </row>
@@ -1979,26 +1978,26 @@
       </c>
     </row>
     <row r="65" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A65" s="7" t="s">
+      <c r="A65" t="s">
         <v>95</v>
       </c>
-      <c r="B65" s="8" t="s">
+      <c r="B65" s="6" t="s">
         <v>97</v>
       </c>
     </row>
     <row r="66" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A66" s="7" t="s">
+      <c r="A66" t="s">
         <v>98</v>
       </c>
-      <c r="B66" s="8" t="s">
+      <c r="B66" s="6" t="s">
         <v>99</v>
       </c>
     </row>
     <row r="67" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A67" s="7" t="s">
+      <c r="A67" t="s">
         <v>100</v>
       </c>
-      <c r="B67" s="8" t="s">
+      <c r="B67" s="6" t="s">
         <v>127</v>
       </c>
     </row>
@@ -2075,257 +2074,242 @@
     <row r="79" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="80" spans="1:3" ht="14.25" customHeight="1">
       <c r="A80" t="s">
-        <v>226</v>
+        <v>349</v>
       </c>
       <c r="B80">
-        <v>30000</v>
+        <v>5</v>
       </c>
       <c r="C80" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="81" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A81" t="s">
-        <v>223</v>
-      </c>
-      <c r="B81">
-        <v>30000</v>
-      </c>
-      <c r="C81" t="s">
-        <v>139</v>
-      </c>
-    </row>
+    <row r="81" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="82" spans="1:3" ht="14.25" customHeight="1">
       <c r="A82" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="B82">
-        <v>60000</v>
+        <v>30000</v>
       </c>
       <c r="C82" t="s">
         <v>139</v>
       </c>
     </row>
     <row r="83" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A83" s="7"/>
-      <c r="B83" s="8"/>
-      <c r="C83" s="7"/>
+      <c r="A83" t="s">
+        <v>223</v>
+      </c>
+      <c r="B83">
+        <v>30000</v>
+      </c>
+      <c r="C83" t="s">
+        <v>139</v>
+      </c>
     </row>
     <row r="84" spans="1:3" ht="14.25" customHeight="1">
       <c r="A84" t="s">
-        <v>145</v>
+        <v>227</v>
       </c>
       <c r="B84">
-        <v>2000</v>
+        <v>60000</v>
       </c>
       <c r="C84" t="s">
         <v>139</v>
       </c>
     </row>
     <row r="85" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A85" t="s">
-        <v>147</v>
-      </c>
-      <c r="B85">
-        <v>10</v>
-      </c>
+      <c r="B85" s="6"/>
     </row>
     <row r="86" spans="1:3" ht="14.25" customHeight="1">
       <c r="A86" t="s">
+        <v>145</v>
+      </c>
+      <c r="B86">
+        <v>2000</v>
+      </c>
+      <c r="C86" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="87" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A87" t="s">
+        <v>147</v>
+      </c>
+      <c r="B87">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="88" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A88" t="s">
         <v>148</v>
       </c>
-      <c r="B86">
+      <c r="B88">
         <v>1</v>
       </c>
-      <c r="C86" t="s">
+      <c r="C88" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="87" spans="1:3" ht="14.25" customHeight="1"/>
-    <row r="88" spans="1:3" ht="15" customHeight="1">
-      <c r="A88" t="s">
+    <row r="89" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="90" spans="1:3" ht="15" customHeight="1">
+      <c r="A90" t="s">
         <v>146</v>
       </c>
-      <c r="B88">
+      <c r="B90">
         <v>2000</v>
       </c>
-      <c r="C88" t="s">
+      <c r="C90" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="89" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A89" t="s">
+    <row r="91" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A91" t="s">
         <v>149</v>
       </c>
-      <c r="B89">
+      <c r="B91">
         <v>10</v>
       </c>
     </row>
-    <row r="90" spans="1:3" ht="17.5" customHeight="1">
-      <c r="A90" t="s">
-        <v>150</v>
-      </c>
-      <c r="B90">
-        <v>1</v>
-      </c>
-      <c r="C90" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="91" spans="1:3" ht="17.5" customHeight="1"/>
     <row r="92" spans="1:3" ht="17.5" customHeight="1">
       <c r="A92" t="s">
-        <v>344</v>
+        <v>150</v>
       </c>
       <c r="B92">
+        <v>1</v>
+      </c>
+      <c r="C92" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="93" spans="1:3" ht="17.5" customHeight="1"/>
+    <row r="94" spans="1:3" ht="17.5" customHeight="1">
+      <c r="A94" t="s">
+        <v>343</v>
+      </c>
+      <c r="B94">
         <v>3000</v>
-      </c>
-      <c r="C92" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="93" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A93" s="7"/>
-      <c r="B93" s="8"/>
-    </row>
-    <row r="94" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A94" s="7" t="s">
-        <v>136</v>
-      </c>
-      <c r="B94" s="8">
-        <v>2000</v>
       </c>
       <c r="C94" t="s">
         <v>139</v>
       </c>
     </row>
     <row r="95" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A95" s="7" t="s">
+      <c r="B95" s="6"/>
+    </row>
+    <row r="96" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A96" t="s">
+        <v>136</v>
+      </c>
+      <c r="B96" s="6">
+        <v>2000</v>
+      </c>
+      <c r="C96" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="97" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A97" t="s">
         <v>138</v>
       </c>
-      <c r="B95">
+      <c r="B97">
         <v>1</v>
       </c>
-      <c r="C95" t="s">
+      <c r="C97" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="96" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A96" s="7" t="s">
+    <row r="98" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A98" t="s">
         <v>140</v>
       </c>
-      <c r="B96" s="8" t="s">
+      <c r="B98" s="6" t="s">
         <v>220</v>
       </c>
-      <c r="C96" s="7"/>
-    </row>
-    <row r="97" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A97" s="7" t="s">
+    </row>
+    <row r="99" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A99" t="s">
         <v>221</v>
       </c>
-      <c r="B97" s="8">
+      <c r="B99" s="6">
         <v>3</v>
       </c>
-      <c r="C97" s="7"/>
-    </row>
-    <row r="98" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A98" s="7" t="s">
-        <v>222</v>
-      </c>
-      <c r="B98" s="8">
-        <v>3</v>
-      </c>
-      <c r="C98" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="99" spans="1:3" ht="14.25" customHeight="1"/>
+    </row>
     <row r="100" spans="1:3" ht="14.25" customHeight="1">
       <c r="A100" t="s">
+        <v>222</v>
+      </c>
+      <c r="B100" s="6">
+        <v>3</v>
+      </c>
+      <c r="C100" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="101" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="102" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A102" t="s">
         <v>241</v>
       </c>
-      <c r="B100" t="s">
+      <c r="B102" t="s">
         <v>242</v>
       </c>
     </row>
-    <row r="101" spans="1:3" ht="14.25" customHeight="1"/>
-    <row r="102" spans="1:3" ht="14" customHeight="1">
-      <c r="A102" t="s">
+    <row r="103" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="104" spans="1:3" ht="14" customHeight="1">
+      <c r="A104" t="s">
         <v>243</v>
       </c>
-      <c r="B102">
+      <c r="B104">
         <v>1</v>
       </c>
-      <c r="C102" t="s">
+      <c r="C104" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="103" spans="1:3" ht="14.25" customHeight="1"/>
-    <row r="104" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A104" t="s">
+    <row r="105" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="106" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A106" t="s">
         <v>249</v>
       </c>
-      <c r="B104" t="s">
+      <c r="B106" t="s">
         <v>248</v>
       </c>
     </row>
-    <row r="105" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A105" t="s">
+    <row r="107" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A107" t="s">
         <v>294</v>
       </c>
-      <c r="B105" t="s">
+      <c r="B107" t="s">
         <v>264</v>
       </c>
     </row>
-    <row r="106" spans="1:3" ht="14.25" customHeight="1"/>
-    <row r="107" spans="1:3" ht="14.25" customHeight="1"/>
-    <row r="108" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A108" t="s">
+    <row r="108" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="109" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="110" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A110" t="s">
         <v>252</v>
       </c>
-      <c r="B108">
+      <c r="B110">
         <v>30000</v>
-      </c>
-      <c r="C108" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="109" spans="1:3" ht="15" customHeight="1">
-      <c r="A109" t="s">
-        <v>255</v>
-      </c>
-      <c r="B109">
-        <v>30000</v>
-      </c>
-      <c r="C109" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="110" spans="1:3" ht="14.5" customHeight="1">
-      <c r="A110" t="s">
-        <v>265</v>
-      </c>
-      <c r="B110">
-        <v>2</v>
       </c>
       <c r="C110" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="111" spans="1:3" ht="14.5" customHeight="1">
+    <row r="111" spans="1:3" ht="15" customHeight="1">
       <c r="A111" t="s">
-        <v>347</v>
+        <v>255</v>
       </c>
       <c r="B111">
-        <v>2</v>
+        <v>30000</v>
       </c>
       <c r="C111" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="112" spans="1:3" ht="15" customHeight="1">
+    <row r="112" spans="1:3" ht="14.5" customHeight="1">
       <c r="A112" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="B112">
         <v>2</v>
@@ -2334,9 +2318,9 @@
         <v>139</v>
       </c>
     </row>
-    <row r="113" spans="1:3" ht="15" customHeight="1">
+    <row r="113" spans="1:3" ht="14.5" customHeight="1">
       <c r="A113" t="s">
-        <v>267</v>
+        <v>346</v>
       </c>
       <c r="B113">
         <v>2</v>
@@ -2347,7 +2331,7 @@
     </row>
     <row r="114" spans="1:3" ht="15" customHeight="1">
       <c r="A114" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="B114">
         <v>2</v>
@@ -2356,9 +2340,9 @@
         <v>139</v>
       </c>
     </row>
-    <row r="115" spans="1:3" ht="14" customHeight="1">
+    <row r="115" spans="1:3" ht="15" customHeight="1">
       <c r="A115" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="B115">
         <v>2</v>
@@ -2367,9 +2351,9 @@
         <v>139</v>
       </c>
     </row>
-    <row r="116" spans="1:3" ht="14" customHeight="1">
+    <row r="116" spans="1:3" ht="15" customHeight="1">
       <c r="A116" t="s">
-        <v>283</v>
+        <v>268</v>
       </c>
       <c r="B116">
         <v>2</v>
@@ -2380,7 +2364,7 @@
     </row>
     <row r="117" spans="1:3" ht="14" customHeight="1">
       <c r="A117" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="B117">
         <v>2</v>
@@ -2391,7 +2375,7 @@
     </row>
     <row r="118" spans="1:3" ht="14" customHeight="1">
       <c r="A118" t="s">
-        <v>271</v>
+        <v>283</v>
       </c>
       <c r="B118">
         <v>2</v>
@@ -2402,7 +2386,7 @@
     </row>
     <row r="119" spans="1:3" ht="14" customHeight="1">
       <c r="A119" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="B119">
         <v>2</v>
@@ -2413,10 +2397,10 @@
     </row>
     <row r="120" spans="1:3" ht="14" customHeight="1">
       <c r="A120" t="s">
-        <v>288</v>
+        <v>271</v>
       </c>
       <c r="B120">
-        <v>3000</v>
+        <v>2</v>
       </c>
       <c r="C120" t="s">
         <v>139</v>
@@ -2424,10 +2408,10 @@
     </row>
     <row r="121" spans="1:3" ht="14" customHeight="1">
       <c r="A121" t="s">
-        <v>291</v>
+        <v>272</v>
       </c>
       <c r="B121">
-        <v>3000</v>
+        <v>2</v>
       </c>
       <c r="C121" t="s">
         <v>139</v>
@@ -2435,7 +2419,7 @@
     </row>
     <row r="122" spans="1:3" ht="14" customHeight="1">
       <c r="A122" t="s">
-        <v>292</v>
+        <v>288</v>
       </c>
       <c r="B122">
         <v>3000</v>
@@ -2446,265 +2430,265 @@
     </row>
     <row r="123" spans="1:3" ht="14" customHeight="1">
       <c r="A123" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="B123">
-        <v>1000</v>
+        <v>3000</v>
       </c>
       <c r="C123" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="124" spans="1:3" ht="14.25" customHeight="1"/>
-    <row r="125" spans="1:3" ht="14.25" customHeight="1"/>
-    <row r="126" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A126" t="s">
-        <v>250</v>
-      </c>
-      <c r="B126" t="s">
-        <v>251</v>
-      </c>
-    </row>
-    <row r="127" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A127" t="s">
-        <v>261</v>
-      </c>
-      <c r="B127" t="s">
-        <v>262</v>
-      </c>
-    </row>
+    <row r="124" spans="1:3" ht="14" customHeight="1">
+      <c r="A124" t="s">
+        <v>292</v>
+      </c>
+      <c r="B124">
+        <v>3000</v>
+      </c>
+      <c r="C124" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="125" spans="1:3" ht="14" customHeight="1">
+      <c r="A125" t="s">
+        <v>293</v>
+      </c>
+      <c r="B125">
+        <v>1000</v>
+      </c>
+      <c r="C125" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="126" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="127" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="128" spans="1:3" ht="14.25" customHeight="1">
       <c r="A128" t="s">
+        <v>250</v>
+      </c>
+      <c r="B128" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="129" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A129" t="s">
+        <v>261</v>
+      </c>
+      <c r="B129" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="130" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A130" t="s">
         <v>259</v>
       </c>
-      <c r="B128" t="s">
+      <c r="B130" t="s">
         <v>260</v>
       </c>
     </row>
-    <row r="129" spans="1:3" ht="14.25" customHeight="1"/>
-    <row r="130" spans="1:3" ht="15" customHeight="1">
-      <c r="A130" t="s">
+    <row r="131" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="132" spans="1:3" ht="15" customHeight="1">
+      <c r="A132" t="s">
         <v>253</v>
       </c>
-      <c r="B130">
+      <c r="B132">
         <v>3</v>
-      </c>
-    </row>
-    <row r="131" spans="1:3" ht="15" customHeight="1">
-      <c r="A131" t="s">
-        <v>254</v>
-      </c>
-      <c r="B131">
-        <v>2</v>
-      </c>
-      <c r="C131" t="s">
-        <v>105</v>
       </c>
     </row>
     <row r="133" spans="1:3" ht="15" customHeight="1">
       <c r="A133" t="s">
-        <v>256</v>
-      </c>
-      <c r="B133" s="16" t="s">
-        <v>276</v>
-      </c>
-    </row>
-    <row r="134" spans="1:3" ht="15" customHeight="1">
-      <c r="A134" t="s">
-        <v>257</v>
-      </c>
-      <c r="B134" s="16" t="s">
-        <v>277</v>
+        <v>254</v>
+      </c>
+      <c r="B133">
+        <v>2</v>
+      </c>
+      <c r="C133" t="s">
+        <v>105</v>
       </c>
     </row>
     <row r="135" spans="1:3" ht="15" customHeight="1">
       <c r="A135" t="s">
-        <v>258</v>
-      </c>
-      <c r="B135" s="16" t="s">
-        <v>278</v>
-      </c>
-    </row>
-    <row r="136" spans="1:3" ht="14.25" customHeight="1">
+        <v>256</v>
+      </c>
+      <c r="B135" s="12" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="136" spans="1:3" ht="15" customHeight="1">
       <c r="A136" t="s">
-        <v>263</v>
-      </c>
-      <c r="B136" s="2" t="s">
-        <v>279</v>
+        <v>257</v>
+      </c>
+      <c r="B136" s="12" t="s">
+        <v>277</v>
       </c>
     </row>
     <row r="137" spans="1:3" ht="15" customHeight="1">
       <c r="A137" t="s">
-        <v>273</v>
-      </c>
-      <c r="B137" s="2" t="s">
-        <v>280</v>
+        <v>258</v>
+      </c>
+      <c r="B137" s="12" t="s">
+        <v>278</v>
       </c>
     </row>
     <row r="138" spans="1:3" ht="14.25" customHeight="1">
       <c r="A138" t="s">
-        <v>274</v>
+        <v>263</v>
       </c>
       <c r="B138" s="2" t="s">
-        <v>285</v>
-      </c>
-    </row>
-    <row r="139" spans="1:3" ht="14.25" customHeight="1">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="139" spans="1:3" ht="15" customHeight="1">
       <c r="A139" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="B139" s="2" t="s">
-        <v>286</v>
+        <v>280</v>
       </c>
     </row>
     <row r="140" spans="1:3" ht="14.25" customHeight="1">
       <c r="A140" t="s">
-        <v>281</v>
-      </c>
-      <c r="B140" t="s">
-        <v>282</v>
+        <v>274</v>
+      </c>
+      <c r="B140" s="2" t="s">
+        <v>285</v>
       </c>
     </row>
     <row r="141" spans="1:3" ht="14.25" customHeight="1">
       <c r="A141" t="s">
-        <v>284</v>
-      </c>
-      <c r="B141" t="s">
-        <v>287</v>
+        <v>275</v>
+      </c>
+      <c r="B141" s="2" t="s">
+        <v>286</v>
       </c>
     </row>
     <row r="142" spans="1:3" ht="14.25" customHeight="1">
       <c r="A142" t="s">
-        <v>289</v>
+        <v>281</v>
       </c>
       <c r="B142" t="s">
-        <v>290</v>
-      </c>
-    </row>
-    <row r="143" spans="1:3" ht="14.25" customHeight="1"/>
+        <v>282</v>
+      </c>
+    </row>
+    <row r="143" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A143" t="s">
+        <v>284</v>
+      </c>
+      <c r="B143" t="s">
+        <v>287</v>
+      </c>
+    </row>
     <row r="144" spans="1:3" ht="14.25" customHeight="1">
       <c r="A144" t="s">
+        <v>289</v>
+      </c>
+      <c r="B144" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="145" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="146" spans="1:2" ht="14.25" customHeight="1">
+      <c r="A146" t="s">
         <v>91</v>
       </c>
-      <c r="B144" t="s">
+      <c r="B146" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="145" spans="1:2" ht="14.25" customHeight="1">
-      <c r="A145" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="146" spans="1:2" ht="14.25" customHeight="1"/>
     <row r="147" spans="1:2" ht="14.25" customHeight="1">
       <c r="A147" t="s">
-        <v>304</v>
-      </c>
-      <c r="B147" t="s">
-        <v>305</v>
-      </c>
-    </row>
-    <row r="148" spans="1:2" ht="14.25" customHeight="1">
-      <c r="A148" t="s">
-        <v>121</v>
-      </c>
-      <c r="B148" t="s">
-        <v>306</v>
-      </c>
-    </row>
+        <v>116</v>
+      </c>
+    </row>
+    <row r="148" spans="1:2" ht="14.25" customHeight="1"/>
     <row r="149" spans="1:2" ht="14.25" customHeight="1">
       <c r="A149" t="s">
-        <v>123</v>
+        <v>304</v>
       </c>
       <c r="B149" t="s">
-        <v>348</v>
-      </c>
-    </row>
-    <row r="150" spans="1:2" ht="14.25" customHeight="1"/>
+        <v>305</v>
+      </c>
+    </row>
+    <row r="150" spans="1:2" ht="14.25" customHeight="1">
+      <c r="A150" t="s">
+        <v>121</v>
+      </c>
+      <c r="B150" t="s">
+        <v>306</v>
+      </c>
+    </row>
     <row r="151" spans="1:2" ht="14.25" customHeight="1">
       <c r="A151" t="s">
+        <v>123</v>
+      </c>
+      <c r="B151" t="s">
+        <v>347</v>
+      </c>
+    </row>
+    <row r="152" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="153" spans="1:2" ht="14.25" customHeight="1">
+      <c r="A153" t="s">
         <v>297</v>
       </c>
-      <c r="B151" t="s">
+      <c r="B153" t="s">
         <v>298</v>
       </c>
     </row>
-    <row r="152" spans="1:2" ht="14.25" customHeight="1">
-      <c r="A152" t="s">
-        <v>299</v>
-      </c>
-      <c r="B152" t="s">
-        <v>300</v>
-      </c>
-    </row>
-    <row r="153" spans="1:2" ht="14.25" customHeight="1"/>
     <row r="154" spans="1:2" ht="14.25" customHeight="1">
       <c r="A154" t="s">
+        <v>299</v>
+      </c>
+      <c r="B154" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="155" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="156" spans="1:2" ht="14.25" customHeight="1">
+      <c r="A156" t="s">
         <v>302</v>
       </c>
-      <c r="B154" t="s">
+      <c r="B156" t="s">
         <v>303</v>
       </c>
     </row>
-    <row r="155" spans="1:2" ht="14.25" customHeight="1">
-      <c r="A155" t="s">
-        <v>301</v>
-      </c>
-      <c r="B155" t="s">
-        <v>300</v>
-      </c>
-    </row>
-    <row r="156" spans="1:2" ht="14.25" customHeight="1"/>
     <row r="157" spans="1:2" ht="14.25" customHeight="1">
       <c r="A157" t="s">
-        <v>107</v>
+        <v>301</v>
       </c>
       <c r="B157" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="158" spans="1:2" ht="14.25" customHeight="1">
-      <c r="A158" t="s">
-        <v>108</v>
-      </c>
-      <c r="B158" t="s">
-        <v>307</v>
-      </c>
-    </row>
+        <v>300</v>
+      </c>
+    </row>
+    <row r="158" spans="1:2" ht="14.25" customHeight="1"/>
     <row r="159" spans="1:2" ht="14.25" customHeight="1">
       <c r="A159" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="B159" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="160" spans="1:2" ht="14.25" customHeight="1"/>
+        <v>106</v>
+      </c>
+    </row>
+    <row r="160" spans="1:2" ht="14.25" customHeight="1">
+      <c r="A160" t="s">
+        <v>108</v>
+      </c>
+      <c r="B160" t="s">
+        <v>348</v>
+      </c>
+    </row>
     <row r="161" spans="1:3" ht="14.25" customHeight="1">
       <c r="A161" t="s">
-        <v>309</v>
-      </c>
-      <c r="B161">
-        <v>60000</v>
-      </c>
-      <c r="C161" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="162" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A162" t="s">
-        <v>308</v>
-      </c>
-      <c r="B162">
-        <v>60000</v>
-      </c>
-      <c r="C162" t="s">
-        <v>139</v>
-      </c>
-    </row>
+        <v>109</v>
+      </c>
+      <c r="B161" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="162" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="163" spans="1:3" ht="14.25" customHeight="1">
       <c r="A163" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="B163">
         <v>60000</v>
@@ -2713,187 +2697,198 @@
         <v>139</v>
       </c>
     </row>
-    <row r="164" spans="1:3" ht="14.25" customHeight="1"/>
-    <row r="165" spans="1:3" s="7" customFormat="1" ht="14.5">
-      <c r="A165" s="7" t="s">
+    <row r="164" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A164" t="s">
+        <v>307</v>
+      </c>
+      <c r="B164">
+        <v>60000</v>
+      </c>
+      <c r="C164" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="165" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A165" t="s">
+        <v>309</v>
+      </c>
+      <c r="B165">
+        <v>60000</v>
+      </c>
+      <c r="C165" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="166" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="167" spans="1:3" ht="14.5">
+      <c r="A167" t="s">
         <v>94</v>
       </c>
-      <c r="B165" s="7" t="s">
+      <c r="B167" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="166" spans="1:3" s="7" customFormat="1" ht="14.5">
-      <c r="A166" s="7" t="s">
+    <row r="168" spans="1:3" ht="14.5">
+      <c r="A168" t="s">
         <v>95</v>
       </c>
-      <c r="B166" s="8" t="s">
+      <c r="B168" s="6" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="167" spans="1:3" s="7" customFormat="1" ht="14.5">
-      <c r="A167" s="7" t="s">
+    <row r="169" spans="1:3" ht="14.5">
+      <c r="A169" t="s">
         <v>98</v>
       </c>
-      <c r="B167" s="8" t="s">
+      <c r="B169" s="6" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="168" spans="1:3" s="7" customFormat="1" ht="14.5">
-      <c r="A168" s="7" t="s">
+    <row r="170" spans="1:3" ht="14.5">
+      <c r="A170" t="s">
         <v>100</v>
       </c>
-      <c r="B168" s="8" t="s">
+      <c r="B170" s="6" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="169" spans="1:3" s="7" customFormat="1" ht="14.5"/>
-    <row r="170" spans="1:3" s="7" customFormat="1" ht="14.5">
-      <c r="A170" s="7" t="s">
+    <row r="171" spans="1:3" ht="14.5"/>
+    <row r="172" spans="1:3" ht="14.5">
+      <c r="A172" t="s">
         <v>101</v>
       </c>
-      <c r="B170" s="8" t="s">
+      <c r="B172" s="6" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="171" spans="1:3" s="7" customFormat="1" ht="14.5">
-      <c r="A171" s="7" t="s">
+    <row r="173" spans="1:3" ht="14.5">
+      <c r="A173" t="s">
         <v>103</v>
       </c>
-      <c r="B171" s="8" t="s">
+      <c r="B173" s="6" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="172" spans="1:3" s="7" customFormat="1" ht="14.5">
-      <c r="A172" s="7" t="s">
+    <row r="174" spans="1:3" ht="14.5">
+      <c r="A174" t="s">
         <v>104</v>
       </c>
-      <c r="B172" s="8">
+      <c r="B174" s="6">
         <v>60</v>
       </c>
-      <c r="C172" s="7" t="s">
+      <c r="C174" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="173" spans="1:3" ht="14.25" customHeight="1"/>
-    <row r="174" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A174" s="7" t="s">
+    <row r="175" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="176" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A176" t="s">
         <v>101</v>
       </c>
-      <c r="B174" s="8" t="s">
+      <c r="B176" s="6" t="s">
         <v>102</v>
       </c>
-      <c r="C174" s="7"/>
-    </row>
-    <row r="175" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A175" s="7" t="s">
+    </row>
+    <row r="177" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A177" t="s">
         <v>103</v>
       </c>
-      <c r="B175" s="9" t="s">
+      <c r="B177" s="7" t="s">
         <v>134</v>
       </c>
-      <c r="C175" s="7"/>
-    </row>
-    <row r="176" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A176" s="7" t="s">
+    </row>
+    <row r="178" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A178" t="s">
         <v>104</v>
       </c>
-      <c r="B176" s="8">
+      <c r="B178" s="6">
         <v>60</v>
       </c>
-      <c r="C176" s="7" t="s">
+      <c r="C178" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="177" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A177" s="7"/>
-      <c r="B177" s="7"/>
-      <c r="C177" s="7"/>
-    </row>
-    <row r="178" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A178" s="7" t="s">
+    <row r="179" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="180" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A180" t="s">
+        <v>311</v>
+      </c>
+      <c r="B180" t="s">
+        <v>320</v>
+      </c>
+      <c r="C180" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="181" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A181" t="s">
         <v>312</v>
       </c>
-      <c r="B178" s="5" t="s">
-        <v>321</v>
-      </c>
-      <c r="C178" s="7" t="s">
+      <c r="B181" s="6" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="182" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A182" t="s">
+        <v>313</v>
+      </c>
+      <c r="B182" s="7" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="183" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A183" t="s">
+        <v>87</v>
+      </c>
+      <c r="C183" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="179" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A179" s="7" t="s">
-        <v>313</v>
-      </c>
-      <c r="B179" s="8" t="s">
-        <v>319</v>
-      </c>
-      <c r="C179" s="7"/>
-    </row>
-    <row r="180" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A180" s="7" t="s">
-        <v>314</v>
-      </c>
-      <c r="B180" s="9" t="s">
-        <v>311</v>
-      </c>
-      <c r="C180" s="7"/>
-    </row>
-    <row r="181" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A181" s="7" t="s">
-        <v>87</v>
-      </c>
-      <c r="B181" s="7"/>
-      <c r="C181" s="7" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="182" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A182" s="7" t="s">
-        <v>88</v>
-      </c>
-      <c r="B182" s="8">
-        <v>60000</v>
-      </c>
-      <c r="C182" s="7" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="183" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="184" spans="1:3" ht="14.25" customHeight="1">
       <c r="A184" t="s">
-        <v>315</v>
-      </c>
-      <c r="B184" s="5" t="s">
-        <v>321</v>
-      </c>
-    </row>
-    <row r="185" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A185" t="s">
-        <v>316</v>
-      </c>
-      <c r="B185" s="8" t="s">
-        <v>318</v>
-      </c>
-    </row>
+        <v>88</v>
+      </c>
+      <c r="B184" s="6">
+        <v>60000</v>
+      </c>
+      <c r="C184" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="185" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="186" spans="1:3" ht="14.25" customHeight="1">
       <c r="A186" t="s">
+        <v>314</v>
+      </c>
+      <c r="B186" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="187" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A187" t="s">
+        <v>315</v>
+      </c>
+      <c r="B187" s="6" t="s">
         <v>317</v>
       </c>
-      <c r="B186" s="9" t="s">
-        <v>320</v>
-      </c>
-    </row>
-    <row r="187" spans="1:3" ht="14.25" customHeight="1"/>
+    </row>
     <row r="188" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A188" s="7" t="s">
+      <c r="A188" t="s">
+        <v>316</v>
+      </c>
+      <c r="B188" s="7" t="s">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="189" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="190" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A190" t="s">
+        <v>321</v>
+      </c>
+      <c r="B190" t="s">
         <v>322</v>
       </c>
-      <c r="B188" t="s">
-        <v>323</v>
-      </c>
-    </row>
-    <row r="189" spans="1:3" ht="14.25" customHeight="1"/>
-    <row r="190" spans="1:3" ht="14.25" customHeight="1"/>
+    </row>
     <row r="191" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="192" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="193" ht="14.25" customHeight="1"/>
@@ -3748,6 +3743,8 @@
     <row r="1042" ht="14.25" customHeight="1"/>
     <row r="1043" ht="14.25" customHeight="1"/>
     <row r="1044" ht="14.25" customHeight="1"/>
+    <row r="1045" ht="14.25" customHeight="1"/>
+    <row r="1046" ht="14.25" customHeight="1"/>
   </sheetData>
   <phoneticPr fontId="3"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -6205,21 +6202,21 @@
       <c r="A27" t="s">
         <v>59</v>
       </c>
-      <c r="B27" s="5" t="s">
+      <c r="B27" t="s">
         <v>60</v>
       </c>
     </row>
     <row r="28" spans="1:2" ht="14.25" customHeight="1">
-      <c r="A28" s="6" t="s">
+      <c r="A28" s="5" t="s">
         <v>62</v>
       </c>
-      <c r="B28" s="6" t="s">
+      <c r="B28" s="5" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="29" spans="1:2" ht="14.25" customHeight="1">
-      <c r="A29" s="6"/>
-      <c r="B29" s="6"/>
+      <c r="A29" s="5"/>
+      <c r="B29" s="5"/>
     </row>
     <row r="30" spans="1:2" ht="14.25" customHeight="1">
       <c r="A30" t="s">
@@ -6303,82 +6300,78 @@
     </row>
     <row r="40" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="41" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A41" s="7" t="s">
+      <c r="A41" t="s">
         <v>83</v>
       </c>
-      <c r="B41" s="5"/>
-      <c r="C41" s="7" t="s">
+      <c r="C41" t="s">
         <v>84</v>
       </c>
     </row>
     <row r="42" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A42" s="7" t="s">
+      <c r="A42" t="s">
         <v>85</v>
       </c>
-      <c r="B42" s="8" t="s">
+      <c r="B42" s="6" t="s">
         <v>128</v>
       </c>
-      <c r="C42" s="7"/>
     </row>
     <row r="43" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A43" s="7" t="s">
+      <c r="A43" t="s">
         <v>86</v>
       </c>
-      <c r="B43" s="9" t="s">
+      <c r="B43" s="7" t="s">
         <v>129</v>
       </c>
-      <c r="C43" s="7"/>
     </row>
     <row r="44" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A44" s="7" t="s">
+      <c r="A44" t="s">
         <v>87</v>
       </c>
-      <c r="B44" s="5"/>
-      <c r="C44" s="7" t="s">
+      <c r="C44" t="s">
         <v>84</v>
       </c>
     </row>
     <row r="45" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A45" s="7" t="s">
+      <c r="A45" t="s">
         <v>88</v>
       </c>
-      <c r="B45" s="8">
+      <c r="B45" s="6">
         <v>10000</v>
       </c>
-      <c r="C45" s="7" t="s">
+      <c r="C45" t="s">
         <v>89</v>
       </c>
     </row>
     <row r="46" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="47" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A47" s="10" t="s">
+      <c r="A47" t="s">
         <v>112</v>
       </c>
-      <c r="B47" s="10" t="s">
+      <c r="B47" t="s">
         <v>61</v>
       </c>
     </row>
     <row r="48" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A48" s="10" t="s">
+      <c r="A48" t="s">
         <v>113</v>
       </c>
-      <c r="B48" s="10" t="s">
+      <c r="B48" t="s">
         <v>125</v>
       </c>
     </row>
     <row r="49" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A49" s="10" t="s">
+      <c r="A49" t="s">
         <v>114</v>
       </c>
-      <c r="B49" s="10" t="s">
+      <c r="B49" t="s">
         <v>126</v>
       </c>
     </row>
     <row r="50" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A50" s="10" t="s">
+      <c r="A50" t="s">
         <v>132</v>
       </c>
-      <c r="B50" s="10" t="s">
+      <c r="B50" t="s">
         <v>133</v>
       </c>
     </row>
@@ -6391,95 +6384,92 @@
       </c>
     </row>
     <row r="52" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A52" s="7" t="s">
+      <c r="A52" t="s">
         <v>95</v>
       </c>
-      <c r="B52" s="8" t="s">
+      <c r="B52" s="6" t="s">
         <v>97</v>
       </c>
     </row>
     <row r="53" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A53" s="7" t="s">
+      <c r="A53" t="s">
         <v>98</v>
       </c>
-      <c r="B53" s="8" t="s">
+      <c r="B53" s="6" t="s">
         <v>99</v>
       </c>
     </row>
     <row r="54" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A54" s="7" t="s">
+      <c r="A54" t="s">
         <v>100</v>
       </c>
-      <c r="B54" s="8" t="s">
+      <c r="B54" s="6" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="55" spans="1:3" s="13" customFormat="1" ht="14.25" customHeight="1">
-      <c r="A55" s="11" t="s">
+    <row r="55" spans="1:3" s="10" customFormat="1" ht="14.25" customHeight="1">
+      <c r="A55" s="8" t="s">
         <v>160</v>
       </c>
-      <c r="B55" s="12" t="s">
+      <c r="B55" s="9" t="s">
         <v>161</v>
       </c>
     </row>
     <row r="56" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A56" s="7"/>
-      <c r="B56" s="8"/>
+      <c r="B56" s="6"/>
     </row>
     <row r="57" spans="1:3" ht="17.5" customHeight="1">
-      <c r="B57" s="8"/>
+      <c r="B57" s="6"/>
     </row>
     <row r="58" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A58" s="7" t="s">
+      <c r="A58" t="s">
         <v>101</v>
       </c>
-      <c r="B58" s="8" t="s">
+      <c r="B58" s="6" t="s">
         <v>102</v>
       </c>
     </row>
     <row r="59" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A59" s="7" t="s">
+      <c r="A59" t="s">
         <v>103</v>
       </c>
-      <c r="B59" s="9" t="s">
+      <c r="B59" s="7" t="s">
         <v>134</v>
       </c>
     </row>
     <row r="60" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A60" s="7" t="s">
+      <c r="A60" t="s">
         <v>104</v>
       </c>
-      <c r="B60" s="8">
+      <c r="B60" s="6">
         <v>60</v>
       </c>
-      <c r="C60" s="7" t="s">
+      <c r="C60" t="s">
         <v>105</v>
       </c>
     </row>
     <row r="61" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="62" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A62" s="7" t="s">
+      <c r="A62" t="s">
         <v>107</v>
       </c>
-      <c r="B62" s="8" t="s">
+      <c r="B62" s="6" t="s">
         <v>106</v>
       </c>
-      <c r="C62" s="7"/>
     </row>
     <row r="63" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A63" s="7" t="s">
+      <c r="A63" t="s">
         <v>108</v>
       </c>
-      <c r="B63" s="8" t="s">
+      <c r="B63" s="6" t="s">
         <v>110</v>
       </c>
-      <c r="C63" s="7"/>
     </row>
     <row r="64" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A64" s="7" t="s">
+      <c r="A64" t="s">
         <v>109</v>
       </c>
-      <c r="B64" s="8" t="s">
+      <c r="B64" s="6" t="s">
         <v>111</v>
       </c>
     </row>
@@ -6648,11 +6638,11 @@
         <v>0</v>
       </c>
     </row>
-    <row r="87" spans="1:2" s="13" customFormat="1" ht="14.25" customHeight="1">
-      <c r="A87" s="13" t="s">
+    <row r="87" spans="1:2" s="10" customFormat="1" ht="14.25" customHeight="1">
+      <c r="A87" s="10" t="s">
         <v>159</v>
       </c>
-      <c r="B87" s="13">
+      <c r="B87" s="10">
         <v>0</v>
       </c>
     </row>

</xml_diff>